<commit_message>
Várias pequenas correções e ajustes. Uso do módulo tempfile para converter mupypdf pximap para qpixmap. Atualização do exemplo.
</commit_message>
<xml_diff>
--- a/docs/example/exemplo.xlsx
+++ b/docs/example/exemplo.xlsx
@@ -25,34 +25,34 @@
     <t xml:space="preserve">Nome</t>
   </si>
   <si>
-    <t xml:space="preserve">Arthur</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Beatriz</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Carlos</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daniela</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Eduardo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fernanda</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Gustavo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Hugo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Isabela</t>
-  </si>
-  <si>
-    <t xml:space="preserve">João</t>
+    <t xml:space="preserve">ARTHUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BEATRIZ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CARLOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DANIELA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EDUARDO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FERNANDA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GUSTAVO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HUGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISABELA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">JOÃO</t>
   </si>
 </sst>
 </file>
@@ -167,7 +167,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>